<commit_message>
started save and load
</commit_message>
<xml_diff>
--- a/Homework 12/Product Backlog.xlsx
+++ b/Homework 12/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/Repositories/1325-repository/Homework 12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4EBE2013-6796-544E-8462-65B795DE31B6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3D019BDE-7359-2A49-9427-7171F7221743}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -660,7 +660,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,13 +679,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -722,8 +715,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +890,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3078,10 +3071,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7222,8 +7215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:J42"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7393,15 +7386,15 @@
       </c>
       <c r="B13">
         <f>C12-D13</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4">
         <f>COUNT(B21:B108)</f>
         <v>28</v>
       </c>
       <c r="D13" s="4">
-        <f>D12</f>
-        <v>19</v>
+        <f>D12+3</f>
+        <v>22</v>
       </c>
       <c r="E13" s="6">
         <v>43219</v>
@@ -8019,7 +8012,7 @@
         <v>19</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="D39" s="4">
         <v>4</v>
@@ -8049,7 +8042,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="D40" s="8">
         <v>5</v>
@@ -9163,7 +9156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="113" workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
@@ -10802,8 +10795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10896,8 +10889,8 @@
         <v>49</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>B10-1</f>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -10906,7 +10899,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -10955,7 +10948,7 @@
         <v>198</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -11075,7 +11068,7 @@
         <v>134</v>
       </c>
       <c r="G23" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -11099,7 +11092,7 @@
         <v>204</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
         <v>178</v>

</xml_diff>